<commit_message>
agregado tests y muevo toda la logica de archivos a un archivo separado
</commit_message>
<xml_diff>
--- a/Pedidos/2021/012020/Pedidos consolidados 01-2021.xlsx
+++ b/Pedidos/2021/012020/Pedidos consolidados 01-2021.xlsx
@@ -1144,7 +1144,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="0" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C2:G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.59375" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -2409,7 +2409,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="topRight" activeCell="C2" activeCellId="0" sqref="C2"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A96" activeCellId="0" sqref="A96"/>
+      <selection pane="bottomRight" activeCell="A96" activeCellId="1" sqref="C2:G44 A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.59375" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="1"/>
@@ -8859,8 +8859,8 @@
   </sheetPr>
   <dimension ref="A1:AO62"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A31" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.59375" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
@@ -9003,17 +9003,29 @@
       </c>
       <c r="C2" s="163" t="inlineStr">
         <is>
-          <t>TIE-G0DXY</t>
+          <t>TIE-WCJGY</t>
         </is>
       </c>
       <c r="D2" s="163" t="inlineStr">
         <is>
-          <t>TIE-IMXAK</t>
-        </is>
-      </c>
-      <c r="E2" s="163" t="n"/>
-      <c r="F2" s="163" t="n"/>
-      <c r="G2" s="163" t="n"/>
+          <t>TIE-VGJ5T</t>
+        </is>
+      </c>
+      <c r="E2" s="163" t="inlineStr">
+        <is>
+          <t>TIE-41ÑTI</t>
+        </is>
+      </c>
+      <c r="F2" s="163" t="inlineStr">
+        <is>
+          <t>TIE-7OÑA1</t>
+        </is>
+      </c>
+      <c r="G2" s="163" t="inlineStr">
+        <is>
+          <t>TIE-ROOBM</t>
+        </is>
+      </c>
       <c r="H2" s="163" t="n"/>
       <c r="I2" s="163" t="n"/>
       <c r="J2" s="163" t="n"/>
@@ -9062,17 +9074,29 @@
       </c>
       <c r="C3" s="113" t="inlineStr">
         <is>
-          <t>Facundo</t>
+          <t>Blas Ingiulla</t>
         </is>
       </c>
       <c r="D3" s="113" t="inlineStr">
         <is>
-          <t>facuhump</t>
-        </is>
-      </c>
-      <c r="E3" s="113" t="n"/>
-      <c r="F3" s="113" t="n"/>
-      <c r="G3" s="113" t="n"/>
+          <t>Luciana lorenzini</t>
+        </is>
+      </c>
+      <c r="E3" s="113" t="inlineStr">
+        <is>
+          <t>Carla Sofía Vargas</t>
+        </is>
+      </c>
+      <c r="F3" s="113" t="inlineStr">
+        <is>
+          <t>*Pablo Buzaglo *</t>
+        </is>
+      </c>
+      <c r="G3" s="113" t="inlineStr">
+        <is>
+          <t>Clara Sepiurca</t>
+        </is>
+      </c>
       <c r="H3" s="113" t="n"/>
       <c r="I3" s="113" t="n"/>
       <c r="J3" s="113" t="n"/>
@@ -9119,17 +9143,29 @@
       </c>
       <c r="C4" s="113" t="inlineStr">
         <is>
-          <t>23/02/2021</t>
+          <t>27/02/2021</t>
         </is>
       </c>
       <c r="D4" s="113" t="inlineStr">
         <is>
-          <t>23/02/2021</t>
-        </is>
-      </c>
-      <c r="E4" s="113" t="n"/>
-      <c r="F4" s="113" t="n"/>
-      <c r="G4" s="113" t="n"/>
+          <t>27/02/2021</t>
+        </is>
+      </c>
+      <c r="E4" s="113" t="inlineStr">
+        <is>
+          <t>27/02/2021</t>
+        </is>
+      </c>
+      <c r="F4" s="113" t="inlineStr">
+        <is>
+          <t>27/02/2021</t>
+        </is>
+      </c>
+      <c r="G4" s="113" t="inlineStr">
+        <is>
+          <t>27/02/2021</t>
+        </is>
+      </c>
       <c r="H4" s="113" t="n"/>
       <c r="I4" s="113" t="n"/>
       <c r="J4" s="113" t="n"/>
@@ -9178,7 +9214,7 @@
       </c>
       <c r="C5" s="113" t="inlineStr">
         <is>
-          <t>24hs</t>
+          <t>Programado</t>
         </is>
       </c>
       <c r="D5" s="113" t="inlineStr">
@@ -9186,9 +9222,21 @@
           <t>Programado</t>
         </is>
       </c>
-      <c r="E5" s="113" t="n"/>
-      <c r="F5" s="113" t="n"/>
-      <c r="G5" s="113" t="n"/>
+      <c r="E5" s="113" t="inlineStr">
+        <is>
+          <t>Programado</t>
+        </is>
+      </c>
+      <c r="F5" s="113" t="inlineStr">
+        <is>
+          <t>Programado</t>
+        </is>
+      </c>
+      <c r="G5" s="113" t="inlineStr">
+        <is>
+          <t>Programado</t>
+        </is>
+      </c>
       <c r="H5" s="113" t="n"/>
       <c r="I5" s="113" t="n"/>
       <c r="J5" s="113" t="n"/>
@@ -9235,7 +9283,7 @@
       </c>
       <c r="C6" s="113" t="inlineStr">
         <is>
-          <t>24/02</t>
+          <t>19/01</t>
         </is>
       </c>
       <c r="D6" s="113" t="inlineStr">
@@ -9243,9 +9291,21 @@
           <t>15/01</t>
         </is>
       </c>
-      <c r="E6" s="113" t="n"/>
-      <c r="F6" s="113" t="n"/>
-      <c r="G6" s="113" t="n"/>
+      <c r="E6" s="113" t="inlineStr">
+        <is>
+          <t>26/01</t>
+        </is>
+      </c>
+      <c r="F6" s="113" t="inlineStr">
+        <is>
+          <t>26/01</t>
+        </is>
+      </c>
+      <c r="G6" s="113" t="inlineStr">
+        <is>
+          <t>26/01</t>
+        </is>
+      </c>
       <c r="H6" s="113" t="n"/>
       <c r="I6" s="113" t="n"/>
       <c r="J6" s="113" t="n"/>
@@ -9345,17 +9405,29 @@
       </c>
       <c r="C8" s="113" t="inlineStr">
         <is>
-          <t>Av. Santa Fé 3000</t>
+          <t>Bauness 2942, Villa Urquiza - Piso 10 Depto B</t>
         </is>
       </c>
       <c r="D8" s="113" t="inlineStr">
         <is>
-          <t>Av. Santa Fé 3000</t>
-        </is>
-      </c>
-      <c r="E8" s="113" t="n"/>
-      <c r="F8" s="113" t="n"/>
-      <c r="G8" s="113" t="n"/>
+          <t>Peña 3028, recoleta-piso 5 Depto A</t>
+        </is>
+      </c>
+      <c r="E8" s="113" t="inlineStr">
+        <is>
+          <t>Av. Indalecio Chenaut 1991 5to piso</t>
+        </is>
+      </c>
+      <c r="F8" s="113" t="inlineStr">
+        <is>
+          <t>Julian Álvarez 687 7 piso</t>
+        </is>
+      </c>
+      <c r="G8" s="113" t="inlineStr">
+        <is>
+          <t>Burela 2040 3º6 - Villa Urquiza</t>
+        </is>
+      </c>
       <c r="H8" s="113" t="n"/>
       <c r="I8" s="113" t="n"/>
       <c r="J8" s="113" t="n"/>
@@ -9412,9 +9484,21 @@
           <t>16 a 20hs</t>
         </is>
       </c>
-      <c r="E9" s="113" t="n"/>
-      <c r="F9" s="113" t="n"/>
-      <c r="G9" s="113" t="n"/>
+      <c r="E9" s="113" t="inlineStr">
+        <is>
+          <t>16 a 20hs</t>
+        </is>
+      </c>
+      <c r="F9" s="113" t="inlineStr">
+        <is>
+          <t>16 a 20hs</t>
+        </is>
+      </c>
+      <c r="G9" s="113" t="inlineStr">
+        <is>
+          <t>16 a 20hs</t>
+        </is>
+      </c>
       <c r="H9" s="113" t="n"/>
       <c r="I9" s="113" t="n"/>
       <c r="J9" s="113" t="n"/>
@@ -9463,17 +9547,29 @@
       </c>
       <c r="C10" s="113" t="inlineStr">
         <is>
-          <t>Transferencia bancaria</t>
+          <t>Mercado Pago</t>
         </is>
       </c>
       <c r="D10" s="113" t="inlineStr">
         <is>
-          <t>Efectivo en la entrega</t>
-        </is>
-      </c>
-      <c r="E10" s="113" t="n"/>
-      <c r="F10" s="113" t="n"/>
-      <c r="G10" s="113" t="n"/>
+          <t>Mercado Pago</t>
+        </is>
+      </c>
+      <c r="E10" s="113" t="inlineStr">
+        <is>
+          <t>Mercado Pago</t>
+        </is>
+      </c>
+      <c r="F10" s="113" t="inlineStr">
+        <is>
+          <t>Mercado Pago</t>
+        </is>
+      </c>
+      <c r="G10" s="113" t="inlineStr">
+        <is>
+          <t>Mercado Pago</t>
+        </is>
+      </c>
       <c r="H10" s="113" t="n"/>
       <c r="I10" s="113" t="n"/>
       <c r="J10" s="113" t="n"/>
@@ -9518,9 +9614,11 @@
       <c r="B11" s="128" t="n">
         <v>2</v>
       </c>
-      <c r="C11" s="128" t="n"/>
+      <c r="C11" s="128" t="n">
+        <v>1</v>
+      </c>
       <c r="D11" s="128" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" s="128" t="n"/>
       <c r="F11" s="128" t="n"/>
@@ -9571,9 +9669,15 @@
       </c>
       <c r="C12" s="128" t="n"/>
       <c r="D12" s="128" t="n"/>
-      <c r="E12" s="128" t="n"/>
-      <c r="F12" s="128" t="n"/>
-      <c r="G12" s="128" t="n"/>
+      <c r="E12" s="128" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="128" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="128" t="n">
+        <v>1</v>
+      </c>
       <c r="H12" s="128" t="n"/>
       <c r="I12" s="128" t="n"/>
       <c r="J12" s="128" t="n"/>
@@ -9668,7 +9772,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="128" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D14" s="128" t="n"/>
       <c r="E14" s="128" t="n"/>
@@ -9721,7 +9825,9 @@
       <c r="C15" s="128" t="n"/>
       <c r="D15" s="128" t="n"/>
       <c r="E15" s="128" t="n"/>
-      <c r="F15" s="128" t="n"/>
+      <c r="F15" s="128" t="n">
+        <v>2</v>
+      </c>
       <c r="G15" s="128" t="n"/>
       <c r="H15" s="128" t="n"/>
       <c r="I15" s="128" t="n"/>
@@ -9866,12 +9972,14 @@
         <v>2</v>
       </c>
       <c r="C18" s="131" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D18" s="131" t="n">
-        <v>4</v>
-      </c>
-      <c r="E18" s="131" t="n"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="131" t="n">
+        <v>1</v>
+      </c>
       <c r="F18" s="131" t="n"/>
       <c r="G18" s="131" t="n"/>
       <c r="H18" s="131" t="n"/>
@@ -9918,8 +10026,12 @@
       <c r="B19" s="131" t="n">
         <v>0</v>
       </c>
-      <c r="C19" s="131" t="n"/>
-      <c r="D19" s="131" t="n"/>
+      <c r="C19" s="131" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="131" t="n">
+        <v>1</v>
+      </c>
       <c r="E19" s="131" t="n"/>
       <c r="F19" s="131" t="n"/>
       <c r="G19" s="131" t="n"/>
@@ -9967,10 +10079,18 @@
       <c r="B20" s="131" t="n">
         <v>0</v>
       </c>
-      <c r="C20" s="131" t="n"/>
-      <c r="D20" s="131" t="n"/>
-      <c r="E20" s="131" t="n"/>
-      <c r="F20" s="131" t="n"/>
+      <c r="C20" s="131" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="131" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="131" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="131" t="n">
+        <v>1</v>
+      </c>
       <c r="G20" s="131" t="n"/>
       <c r="H20" s="131" t="n"/>
       <c r="I20" s="131" t="n"/>
@@ -10065,11 +10185,17 @@
       <c r="B22" s="131" t="n">
         <v>6</v>
       </c>
-      <c r="C22" s="131" t="n"/>
+      <c r="C22" s="131" t="n">
+        <v>1</v>
+      </c>
       <c r="D22" s="131" t="n"/>
-      <c r="E22" s="131" t="n"/>
+      <c r="E22" s="131" t="n">
+        <v>2</v>
+      </c>
       <c r="F22" s="131" t="n"/>
-      <c r="G22" s="131" t="n"/>
+      <c r="G22" s="131" t="n">
+        <v>1</v>
+      </c>
       <c r="H22" s="131" t="n"/>
       <c r="I22" s="131" t="n"/>
       <c r="J22" s="131" t="n"/>
@@ -10114,13 +10240,17 @@
       <c r="B23" s="131" t="n">
         <v>2</v>
       </c>
-      <c r="C23" s="131" t="n"/>
+      <c r="C23" s="131" t="n">
+        <v>1</v>
+      </c>
       <c r="D23" s="131" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E23" s="131" t="n"/>
       <c r="F23" s="131" t="n"/>
-      <c r="G23" s="131" t="n"/>
+      <c r="G23" s="131" t="n">
+        <v>1</v>
+      </c>
       <c r="H23" s="131" t="n"/>
       <c r="I23" s="131" t="n"/>
       <c r="J23" s="131" t="n"/>
@@ -10165,8 +10295,12 @@
       <c r="B24" s="131" t="n">
         <v>0</v>
       </c>
-      <c r="C24" s="131" t="n"/>
-      <c r="D24" s="131" t="n"/>
+      <c r="C24" s="131" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="131" t="n">
+        <v>1</v>
+      </c>
       <c r="E24" s="131" t="n"/>
       <c r="F24" s="131" t="n"/>
       <c r="G24" s="131" t="n"/>
@@ -10413,7 +10547,9 @@
       <c r="C29" s="115" t="n"/>
       <c r="D29" s="115" t="n"/>
       <c r="E29" s="115" t="n"/>
-      <c r="F29" s="115" t="n"/>
+      <c r="F29" s="115" t="n">
+        <v>1</v>
+      </c>
       <c r="G29" s="115" t="n"/>
       <c r="H29" s="115" t="n"/>
       <c r="I29" s="115" t="n"/>
@@ -10658,7 +10794,9 @@
       <c r="C34" s="115" t="n"/>
       <c r="D34" s="115" t="n"/>
       <c r="E34" s="115" t="n"/>
-      <c r="F34" s="115" t="n"/>
+      <c r="F34" s="115" t="n">
+        <v>1</v>
+      </c>
       <c r="G34" s="115" t="n"/>
       <c r="H34" s="115" t="n"/>
       <c r="I34" s="115" t="n"/>
@@ -10852,7 +10990,7 @@
         <v>9</v>
       </c>
       <c r="C38" s="143" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D38" s="143" t="n"/>
       <c r="E38" s="143" t="n"/>
@@ -10902,10 +11040,10 @@
       <c r="B39" s="143" t="n">
         <v>0</v>
       </c>
-      <c r="C39" s="143" t="n"/>
-      <c r="D39" s="143" t="n">
-        <v>10</v>
-      </c>
+      <c r="C39" s="143" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" s="143" t="n"/>
       <c r="E39" s="143" t="n"/>
       <c r="F39" s="143" t="n"/>
       <c r="G39" s="143" t="n"/>
@@ -10953,11 +11091,17 @@
       <c r="B40" s="143" t="n">
         <v>0</v>
       </c>
-      <c r="C40" s="143" t="n"/>
-      <c r="D40" s="143" t="n"/>
+      <c r="C40" s="143" t="n">
+        <v>2</v>
+      </c>
+      <c r="D40" s="143" t="n">
+        <v>1</v>
+      </c>
       <c r="E40" s="143" t="n"/>
       <c r="F40" s="143" t="n"/>
-      <c r="G40" s="143" t="n"/>
+      <c r="G40" s="143" t="n">
+        <v>1</v>
+      </c>
       <c r="H40" s="143" t="n"/>
       <c r="I40" s="143" t="n"/>
       <c r="J40" s="143" t="n"/>
@@ -11003,10 +11147,18 @@
         <v>0</v>
       </c>
       <c r="C41" s="143" t="n"/>
-      <c r="D41" s="143" t="n"/>
-      <c r="E41" s="143" t="n"/>
-      <c r="F41" s="143" t="n"/>
-      <c r="G41" s="143" t="n"/>
+      <c r="D41" s="143" t="n">
+        <v>2</v>
+      </c>
+      <c r="E41" s="143" t="n">
+        <v>2</v>
+      </c>
+      <c r="F41" s="143" t="n">
+        <v>2</v>
+      </c>
+      <c r="G41" s="143" t="n">
+        <v>2</v>
+      </c>
       <c r="H41" s="143" t="n"/>
       <c r="I41" s="143" t="n"/>
       <c r="J41" s="143" t="n"/>
@@ -11054,8 +11206,12 @@
       <c r="C42" s="143" t="n"/>
       <c r="D42" s="143" t="n"/>
       <c r="E42" s="143" t="n"/>
-      <c r="F42" s="143" t="n"/>
-      <c r="G42" s="143" t="n"/>
+      <c r="F42" s="143" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="143" t="n">
+        <v>1</v>
+      </c>
       <c r="H42" s="143" t="n"/>
       <c r="I42" s="143" t="n"/>
       <c r="J42" s="143" t="n"/>
@@ -11100,9 +11256,15 @@
       <c r="B43" s="143" t="n">
         <v>0</v>
       </c>
-      <c r="C43" s="143" t="n"/>
-      <c r="D43" s="143" t="n"/>
-      <c r="E43" s="143" t="n"/>
+      <c r="C43" s="143" t="n">
+        <v>2</v>
+      </c>
+      <c r="D43" s="143" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" s="143" t="n">
+        <v>1</v>
+      </c>
       <c r="F43" s="143" t="n"/>
       <c r="G43" s="143" t="n"/>
       <c r="H43" s="143" t="n"/>
@@ -11150,8 +11312,12 @@
         <v>0</v>
       </c>
       <c r="C44" s="143" t="n"/>
-      <c r="D44" s="143" t="n"/>
-      <c r="E44" s="143" t="n"/>
+      <c r="D44" s="143" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" s="143" t="n">
+        <v>3</v>
+      </c>
       <c r="F44" s="143" t="n"/>
       <c r="G44" s="143" t="n"/>
       <c r="H44" s="143" t="n"/>
@@ -12087,7 +12253,7 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:G44 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.59375" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
@@ -12111,7 +12277,7 @@
   <dimension ref="A1:Y49"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="0" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+      <selection pane="topLeft" activeCell="I25" activeCellId="1" sqref="C2:G44 I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.59375" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>

</xml_diff>